<commit_message>
Added data source description for year 2003 data in the excel file. No need to change the Taiwan emissions inventory processing code in module-E.
</commit_message>
<xml_diff>
--- a/input/emissions-inventories/Taiwan/Taiwan_emissions.xlsx
+++ b/input/emissions-inventories/Taiwan/Taiwan_emissions.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="160">
   <si>
-    <t>Unit: Metric tonnes/yr</t>
-  </si>
-  <si>
     <t>Sector</t>
   </si>
   <si>
@@ -499,6 +496,9 @@
   </si>
   <si>
     <t>Non-ferrous metal products</t>
+  </si>
+  <si>
+    <t>Source: Taiwan EPA Report: EPA-95-FA11-03-D067; Unit: Metric tonnes/yr</t>
   </si>
 </sst>
 </file>
@@ -3269,49 +3269,49 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" t="s">
         <v>122</v>
-      </c>
-      <c r="D1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
         <v>117</v>
-      </c>
-      <c r="B2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" t="s">
         <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="B5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="1">
         <v>321000</v>
       </c>
       <c r="F5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G5" s="1">
         <v>235000</v>
       </c>
       <c r="J5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K5" s="1">
         <v>490000</v>
@@ -3319,36 +3319,36 @@
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" t="s">
         <v>125</v>
       </c>
-      <c r="D7" t="s">
-        <v>126</v>
-      </c>
       <c r="F7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" t="s">
         <v>125</v>
       </c>
-      <c r="H7" t="s">
-        <v>126</v>
-      </c>
       <c r="J7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" t="s">
+        <v>124</v>
+      </c>
+      <c r="L7" t="s">
         <v>125</v>
-      </c>
-      <c r="L7" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="B8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="2">
         <v>0.28999999999999998</v>
@@ -3357,7 +3357,7 @@
         <v>93090</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G8" s="2">
         <v>0.36</v>
@@ -3366,7 +3366,7 @@
         <v>84600</v>
       </c>
       <c r="J8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K8" s="2">
         <v>0.25</v>
@@ -3377,7 +3377,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="B9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C9" s="2">
         <v>0.04</v>
@@ -3386,7 +3386,7 @@
         <v>12840</v>
       </c>
       <c r="F9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G9" s="2">
         <v>0.19</v>
@@ -3395,7 +3395,7 @@
         <v>44650</v>
       </c>
       <c r="J9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K9" s="2">
         <v>0.2</v>
@@ -3406,7 +3406,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C10" s="2">
         <v>7.0000000000000007E-2</v>
@@ -3415,7 +3415,7 @@
         <v>22470</v>
       </c>
       <c r="F10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G10" s="2">
         <v>0.35</v>
@@ -3424,7 +3424,7 @@
         <v>82250</v>
       </c>
       <c r="J10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K10" s="2">
         <v>0.23</v>
@@ -3435,7 +3435,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="B11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C11" s="2">
         <v>7.0000000000000007E-2</v>
@@ -3444,7 +3444,7 @@
         <v>22470</v>
       </c>
       <c r="F11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G11" s="2">
         <v>0.02</v>
@@ -3453,7 +3453,7 @@
         <v>4700</v>
       </c>
       <c r="J11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K11" s="2">
         <v>0.03</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C12" s="2">
         <v>7.0000000000000007E-2</v>
@@ -3473,7 +3473,7 @@
         <v>22470</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G12" s="2">
         <v>0.08</v>
@@ -3482,7 +3482,7 @@
         <v>18800</v>
       </c>
       <c r="J12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K12" s="2">
         <v>0.04</v>
@@ -3493,7 +3493,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2">
         <v>0.05</v>
@@ -3502,7 +3502,7 @@
         <v>16050</v>
       </c>
       <c r="J13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K13" s="2">
         <v>0.2</v>
@@ -3513,7 +3513,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="B14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C14" s="2">
         <v>0.24</v>
@@ -3522,7 +3522,7 @@
         <v>77040</v>
       </c>
       <c r="J14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K14" s="2">
         <v>0.05</v>
@@ -3533,7 +3533,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="B15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2">
         <v>0.14000000000000001</v>
@@ -3544,7 +3544,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="B16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" s="2">
         <v>0.03</v>
@@ -3555,30 +3555,30 @@
     </row>
     <row r="18" spans="2:12">
       <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
         <v>8</v>
       </c>
-      <c r="F18" t="s">
-        <v>9</v>
-      </c>
       <c r="J18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:12">
       <c r="B19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C19" s="1">
         <v>889000</v>
       </c>
       <c r="F19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G19" s="1">
         <v>1104000</v>
       </c>
       <c r="J19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K19" s="1">
         <v>1104000</v>
@@ -3586,36 +3586,36 @@
     </row>
     <row r="21" spans="2:12">
       <c r="B21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" t="s">
         <v>125</v>
       </c>
-      <c r="D21" t="s">
-        <v>126</v>
-      </c>
       <c r="F21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="s">
+        <v>124</v>
+      </c>
+      <c r="H21" t="s">
         <v>125</v>
       </c>
-      <c r="H21" t="s">
-        <v>126</v>
-      </c>
       <c r="J21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" t="s">
+        <v>124</v>
+      </c>
+      <c r="L21" t="s">
         <v>125</v>
-      </c>
-      <c r="L21" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="22" spans="2:12">
       <c r="B22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C22" s="2">
         <v>0.11</v>
@@ -3624,7 +3624,7 @@
         <v>97790</v>
       </c>
       <c r="F22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G22" s="2">
         <v>0.56000000000000005</v>
@@ -3633,7 +3633,7 @@
         <v>618240</v>
       </c>
       <c r="J22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K22" s="2">
         <v>0.02</v>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="23" spans="2:12">
       <c r="B23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C23" s="2">
         <v>0.11</v>
@@ -3653,7 +3653,7 @@
         <v>35310</v>
       </c>
       <c r="F23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G23" s="2">
         <v>0.15</v>
@@ -3662,7 +3662,7 @@
         <v>165600</v>
       </c>
       <c r="J23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K23" s="2">
         <v>0.16</v>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="24" spans="2:12">
       <c r="B24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C24" s="2">
         <v>0.09</v>
@@ -3682,7 +3682,7 @@
         <v>28890</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G24" s="2">
         <v>0.04</v>
@@ -3691,7 +3691,7 @@
         <v>44160</v>
       </c>
       <c r="J24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K24" s="2">
         <v>0.82</v>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="25" spans="2:12">
       <c r="B25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" s="2">
         <v>0.12</v>
@@ -3711,7 +3711,7 @@
         <v>38520</v>
       </c>
       <c r="F25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G25" s="2">
         <v>0.16</v>
@@ -3722,7 +3722,7 @@
     </row>
     <row r="26" spans="2:12">
       <c r="B26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" s="2">
         <v>0.17</v>
@@ -3731,7 +3731,7 @@
         <v>54570</v>
       </c>
       <c r="F26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G26" s="2">
         <v>7.0000000000000007E-2</v>
@@ -3742,7 +3742,7 @@
     </row>
     <row r="27" spans="2:12">
       <c r="B27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C27" s="2">
         <v>0.1</v>
@@ -3751,7 +3751,7 @@
         <v>32100</v>
       </c>
       <c r="F27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G27" s="2">
         <v>0.02</v>
@@ -3762,7 +3762,7 @@
     </row>
     <row r="28" spans="2:12">
       <c r="B28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C28" s="2">
         <v>0.15</v>
@@ -3773,7 +3773,7 @@
     </row>
     <row r="29" spans="2:12">
       <c r="B29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" s="2">
         <v>0.15</v>
@@ -3791,64 +3791,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
         <v>115</v>
       </c>
-      <c r="B3" t="s">
-        <v>116</v>
-      </c>
       <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
         <v>113</v>
       </c>
-      <c r="D3" t="s">
-        <v>114</v>
-      </c>
       <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
       <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" t="s">
         <v>8</v>
       </c>
-      <c r="K3" t="s">
-        <v>9</v>
-      </c>
       <c r="L3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>54</v>
-      </c>
-      <c r="C4" t="s">
-        <v>55</v>
       </c>
       <c r="E4">
         <v>9621</v>
@@ -3877,13 +3875,13 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
         <v>53</v>
       </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5">
         <v>1727</v>
@@ -3912,13 +3910,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
         <v>53</v>
       </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6">
         <v>9095</v>
@@ -3947,13 +3945,13 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" t="s">
-        <v>54</v>
-      </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7">
         <v>1114</v>
@@ -3982,13 +3980,13 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
         <v>53</v>
       </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8">
         <v>9681</v>
@@ -4017,13 +4015,13 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
         <v>53</v>
       </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9">
         <v>25867</v>
@@ -4052,13 +4050,13 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
         <v>53</v>
       </c>
-      <c r="B10" t="s">
-        <v>54</v>
-      </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10">
         <v>8712</v>
@@ -4087,13 +4085,13 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s">
-        <v>54</v>
-      </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -4122,13 +4120,13 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
         <v>53</v>
       </c>
-      <c r="B12" t="s">
-        <v>54</v>
-      </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12">
         <v>1650</v>
@@ -4157,13 +4155,13 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
-        <v>54</v>
-      </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13">
         <v>1020</v>
@@ -4192,13 +4190,13 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E14">
         <v>20383</v>
@@ -4227,13 +4225,13 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
         <v>53</v>
       </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15">
         <v>4478</v>
@@ -4262,13 +4260,13 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
         <v>53</v>
       </c>
-      <c r="B16" t="s">
-        <v>54</v>
-      </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16">
         <v>1438</v>
@@ -4297,13 +4295,13 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
         <v>53</v>
       </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17">
         <v>9406</v>
@@ -4332,13 +4330,13 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" t="s">
-        <v>54</v>
-      </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18">
         <v>122</v>
@@ -4367,13 +4365,13 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
         <v>53</v>
       </c>
-      <c r="B19" t="s">
-        <v>54</v>
-      </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19">
         <v>2508</v>
@@ -4402,13 +4400,13 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
         <v>53</v>
       </c>
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20">
         <v>2065</v>
@@ -4437,13 +4435,13 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
         <v>53</v>
       </c>
-      <c r="B21" t="s">
-        <v>54</v>
-      </c>
       <c r="C21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E21">
         <v>1320</v>
@@ -4472,13 +4470,13 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
         <v>53</v>
       </c>
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22">
         <v>34643</v>
@@ -4507,13 +4505,13 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
         <v>53</v>
       </c>
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E23">
         <v>1700</v>
@@ -4542,13 +4540,13 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
         <v>53</v>
       </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E24">
         <v>501</v>
@@ -4577,13 +4575,13 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="B25" t="s">
-        <v>54</v>
-      </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E25">
         <v>2150</v>
@@ -4612,13 +4610,13 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
         <v>53</v>
       </c>
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E26">
         <v>401</v>
@@ -4647,13 +4645,13 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
         <v>53</v>
       </c>
-      <c r="B27" t="s">
-        <v>54</v>
-      </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4682,13 +4680,13 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
         <v>53</v>
       </c>
-      <c r="B28" t="s">
-        <v>54</v>
-      </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -4717,13 +4715,13 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
         <v>53</v>
       </c>
-      <c r="B29" t="s">
-        <v>54</v>
-      </c>
       <c r="C29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -4752,13 +4750,13 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
         <v>53</v>
       </c>
-      <c r="B30" t="s">
-        <v>54</v>
-      </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -4787,13 +4785,13 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" t="s">
         <v>53</v>
       </c>
-      <c r="B31" t="s">
-        <v>54</v>
-      </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -4822,13 +4820,13 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
         <v>53</v>
       </c>
-      <c r="B32" t="s">
-        <v>54</v>
-      </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -4857,13 +4855,13 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" t="s">
         <v>53</v>
       </c>
-      <c r="B33" t="s">
-        <v>54</v>
-      </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -4892,13 +4890,13 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" t="s">
         <v>53</v>
       </c>
-      <c r="B34" t="s">
-        <v>54</v>
-      </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E34">
         <v>18051</v>
@@ -4927,13 +4925,13 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
         <v>77</v>
-      </c>
-      <c r="C35" t="s">
-        <v>78</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -4962,13 +4960,13 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -4997,13 +4995,13 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -5032,13 +5030,13 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -5067,13 +5065,13 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E39">
         <v>9</v>
@@ -5102,13 +5100,13 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E40">
         <v>5686</v>
@@ -5137,13 +5135,13 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E41">
         <v>62</v>
@@ -5172,13 +5170,13 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E42">
         <v>1323</v>
@@ -5207,13 +5205,13 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E43">
         <v>52538</v>
@@ -5242,13 +5240,13 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -5277,13 +5275,13 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -5312,13 +5310,13 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -5347,13 +5345,13 @@
     </row>
     <row r="47" spans="1:12">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E47">
         <v>370287</v>
@@ -5382,13 +5380,13 @@
     </row>
     <row r="48" spans="1:12">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E48">
         <v>77020</v>
@@ -5417,13 +5415,13 @@
     </row>
     <row r="49" spans="1:12">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E49">
         <v>41840</v>
@@ -5452,13 +5450,13 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E50">
         <v>10226</v>
@@ -5484,10 +5482,10 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E51">
         <v>209</v>
@@ -5516,10 +5514,10 @@
     </row>
     <row r="52" spans="1:12">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E52">
         <v>351</v>
@@ -5548,13 +5546,13 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" t="s">
         <v>94</v>
-      </c>
-      <c r="C53" t="s">
-        <v>95</v>
       </c>
       <c r="E53">
         <v>2286</v>
@@ -5583,13 +5581,13 @@
     </row>
     <row r="54" spans="1:12">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E54">
         <v>42</v>
@@ -5618,13 +5616,13 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C55" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E55">
         <v>2963</v>
@@ -5653,13 +5651,13 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C56" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E56">
         <v>49</v>
@@ -5688,10 +5686,10 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -5720,10 +5718,10 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E58">
         <v>2594</v>
@@ -5752,16 +5750,16 @@
     </row>
     <row r="59" spans="1:12">
       <c r="A59" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" t="s">
+        <v>42</v>
+      </c>
+      <c r="C59" t="s">
         <v>98</v>
       </c>
-      <c r="B59" t="s">
-        <v>43</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>99</v>
-      </c>
-      <c r="D59" t="s">
-        <v>100</v>
       </c>
       <c r="E59">
         <v>11036</v>
@@ -5790,16 +5788,16 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" t="s">
+        <v>42</v>
+      </c>
+      <c r="C60" t="s">
         <v>98</v>
       </c>
-      <c r="B60" t="s">
-        <v>43</v>
-      </c>
-      <c r="C60" t="s">
-        <v>99</v>
-      </c>
       <c r="D60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E60">
         <v>574</v>
@@ -5828,16 +5826,16 @@
     </row>
     <row r="61" spans="1:12">
       <c r="A61" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" t="s">
         <v>98</v>
       </c>
-      <c r="B61" t="s">
-        <v>43</v>
-      </c>
-      <c r="C61" t="s">
-        <v>99</v>
-      </c>
       <c r="D61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E61">
         <v>1437</v>
@@ -5866,16 +5864,16 @@
     </row>
     <row r="62" spans="1:12">
       <c r="A62" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C62" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D62" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E62">
         <v>1685</v>
@@ -5904,16 +5902,16 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C63" t="s">
+        <v>102</v>
+      </c>
+      <c r="D63" t="s">
         <v>103</v>
-      </c>
-      <c r="D63" t="s">
-        <v>104</v>
       </c>
       <c r="E63">
         <v>1366</v>
@@ -5942,16 +5940,16 @@
     </row>
     <row r="64" spans="1:12">
       <c r="A64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C64" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D64" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E64">
         <v>2875</v>
@@ -5980,16 +5978,16 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C65" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D65" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E65">
         <v>14053</v>
@@ -6018,16 +6016,16 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C66" t="s">
+        <v>106</v>
+      </c>
+      <c r="D66" t="s">
         <v>107</v>
-      </c>
-      <c r="D66" t="s">
-        <v>108</v>
       </c>
       <c r="E66">
         <v>5746</v>
@@ -6056,16 +6054,16 @@
     </row>
     <row r="67" spans="1:12">
       <c r="A67" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C67" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D67" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E67">
         <v>2340</v>
@@ -6094,13 +6092,13 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B68" t="s">
+        <v>109</v>
+      </c>
+      <c r="C68" t="s">
         <v>110</v>
-      </c>
-      <c r="C68" t="s">
-        <v>111</v>
       </c>
       <c r="E68">
         <v>148</v>
@@ -6129,13 +6127,13 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B69" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C69" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E69">
         <v>122</v>
@@ -6164,13 +6162,13 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B70" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C70" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -6199,13 +6197,13 @@
     </row>
     <row r="71" spans="1:12">
       <c r="A71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B71" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C71" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E71">
         <v>453</v>
@@ -6241,64 +6239,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
         <v>115</v>
       </c>
-      <c r="B3" t="s">
-        <v>116</v>
-      </c>
       <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
         <v>113</v>
       </c>
-      <c r="D3" t="s">
-        <v>114</v>
-      </c>
       <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
       <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" t="s">
         <v>8</v>
       </c>
-      <c r="K3" t="s">
-        <v>9</v>
-      </c>
       <c r="L3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>54</v>
-      </c>
-      <c r="C4" t="s">
-        <v>55</v>
       </c>
       <c r="E4">
         <v>6319</v>
@@ -6327,13 +6323,13 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
         <v>53</v>
       </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5">
         <v>1488</v>
@@ -6362,13 +6358,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
         <v>53</v>
       </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6">
         <v>4030</v>
@@ -6397,13 +6393,13 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" t="s">
-        <v>54</v>
-      </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7">
         <v>835</v>
@@ -6432,13 +6428,13 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
         <v>53</v>
       </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8">
         <v>12233</v>
@@ -6467,13 +6463,13 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
         <v>53</v>
       </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9">
         <v>13353</v>
@@ -6502,13 +6498,13 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
         <v>53</v>
       </c>
-      <c r="B10" t="s">
-        <v>54</v>
-      </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10">
         <v>3282</v>
@@ -6537,13 +6533,13 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s">
-        <v>54</v>
-      </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -6572,13 +6568,13 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
         <v>53</v>
       </c>
-      <c r="B12" t="s">
-        <v>54</v>
-      </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12">
         <v>958</v>
@@ -6607,13 +6603,13 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
-        <v>54</v>
-      </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13">
         <v>382</v>
@@ -6642,13 +6638,13 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E14">
         <v>8173</v>
@@ -6677,13 +6673,13 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
         <v>53</v>
       </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15">
         <v>2175</v>
@@ -6712,13 +6708,13 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
         <v>53</v>
       </c>
-      <c r="B16" t="s">
-        <v>54</v>
-      </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16">
         <v>1128</v>
@@ -6747,13 +6743,13 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
         <v>53</v>
       </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17">
         <v>4102</v>
@@ -6782,13 +6778,13 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" t="s">
-        <v>54</v>
-      </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18">
         <v>94</v>
@@ -6817,13 +6813,13 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
         <v>53</v>
       </c>
-      <c r="B19" t="s">
-        <v>54</v>
-      </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19">
         <v>1756</v>
@@ -6852,13 +6848,13 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
         <v>53</v>
       </c>
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20">
         <v>1255</v>
@@ -6887,13 +6883,13 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
         <v>53</v>
       </c>
-      <c r="B21" t="s">
-        <v>54</v>
-      </c>
       <c r="C21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E21">
         <v>1136</v>
@@ -6922,13 +6918,13 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
         <v>53</v>
       </c>
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22">
         <v>17640</v>
@@ -6957,13 +6953,13 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
         <v>53</v>
       </c>
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E23">
         <v>973</v>
@@ -6992,13 +6988,13 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
         <v>53</v>
       </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E24">
         <v>313</v>
@@ -7027,13 +7023,13 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="B25" t="s">
-        <v>54</v>
-      </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E25">
         <v>895</v>
@@ -7062,13 +7058,13 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
         <v>53</v>
       </c>
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E26">
         <v>80</v>
@@ -7097,13 +7093,13 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
         <v>53</v>
       </c>
-      <c r="B27" t="s">
-        <v>54</v>
-      </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E27">
         <v>211</v>
@@ -7132,13 +7128,13 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
         <v>53</v>
       </c>
-      <c r="B28" t="s">
-        <v>54</v>
-      </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -7167,13 +7163,13 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
         <v>53</v>
       </c>
-      <c r="B29" t="s">
-        <v>54</v>
-      </c>
       <c r="C29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -7202,13 +7198,13 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
         <v>53</v>
       </c>
-      <c r="B30" t="s">
-        <v>54</v>
-      </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -7237,13 +7233,13 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" t="s">
         <v>53</v>
       </c>
-      <c r="B31" t="s">
-        <v>54</v>
-      </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -7272,13 +7268,13 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
         <v>53</v>
       </c>
-      <c r="B32" t="s">
-        <v>54</v>
-      </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -7307,13 +7303,13 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" t="s">
         <v>53</v>
       </c>
-      <c r="B33" t="s">
-        <v>54</v>
-      </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -7342,13 +7338,13 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" t="s">
         <v>53</v>
       </c>
-      <c r="B34" t="s">
-        <v>54</v>
-      </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E34">
         <v>11616</v>
@@ -7377,13 +7373,13 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
         <v>77</v>
-      </c>
-      <c r="C35" t="s">
-        <v>78</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -7412,13 +7408,13 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -7447,13 +7443,13 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -7482,13 +7478,13 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -7517,13 +7513,13 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -7552,13 +7548,13 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E40">
         <v>6517</v>
@@ -7587,13 +7583,13 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E41">
         <v>50</v>
@@ -7622,13 +7618,13 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E42">
         <v>737</v>
@@ -7657,13 +7653,13 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E43">
         <v>63329</v>
@@ -7692,13 +7688,13 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -7727,13 +7723,13 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -7762,13 +7758,13 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -7797,13 +7793,13 @@
     </row>
     <row r="47" spans="1:12">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E47">
         <v>345001</v>
@@ -7832,13 +7828,13 @@
     </row>
     <row r="48" spans="1:12">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E48">
         <v>65534</v>
@@ -7867,13 +7863,13 @@
     </row>
     <row r="49" spans="1:12">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E49">
         <v>12947</v>
@@ -7902,13 +7898,13 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E50">
         <v>24543</v>
@@ -7937,13 +7933,13 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E51">
         <v>15607</v>
@@ -7972,10 +7968,10 @@
     </row>
     <row r="52" spans="1:12">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E52">
         <v>214</v>
@@ -8004,10 +8000,10 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E53">
         <v>631</v>
@@ -8036,13 +8032,13 @@
     </row>
     <row r="54" spans="1:12">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" t="s">
         <v>94</v>
-      </c>
-      <c r="C54" t="s">
-        <v>95</v>
       </c>
       <c r="E54">
         <v>1966</v>
@@ -8071,13 +8067,13 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E55">
         <v>24</v>
@@ -8106,13 +8102,13 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E56">
         <v>2435</v>
@@ -8141,13 +8137,13 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E57">
         <v>22</v>
@@ -8176,10 +8172,10 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -8208,10 +8204,10 @@
     </row>
     <row r="59" spans="1:12">
       <c r="A59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B59" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E59">
         <v>587</v>
@@ -8240,16 +8236,16 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" t="s">
+        <v>42</v>
+      </c>
+      <c r="C60" t="s">
         <v>98</v>
       </c>
-      <c r="B60" t="s">
-        <v>43</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>99</v>
-      </c>
-      <c r="D60" t="s">
-        <v>100</v>
       </c>
       <c r="E60">
         <v>9633</v>
@@ -8278,16 +8274,16 @@
     </row>
     <row r="61" spans="1:12">
       <c r="A61" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" t="s">
         <v>98</v>
       </c>
-      <c r="B61" t="s">
-        <v>43</v>
-      </c>
-      <c r="C61" t="s">
-        <v>99</v>
-      </c>
       <c r="D61" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E61">
         <v>600</v>
@@ -8316,16 +8312,16 @@
     </row>
     <row r="62" spans="1:12">
       <c r="A62" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" t="s">
+        <v>42</v>
+      </c>
+      <c r="C62" t="s">
         <v>98</v>
       </c>
-      <c r="B62" t="s">
-        <v>43</v>
-      </c>
-      <c r="C62" t="s">
-        <v>99</v>
-      </c>
       <c r="D62" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E62">
         <v>1418</v>
@@ -8354,16 +8350,16 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C63" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D63" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E63">
         <v>1558</v>
@@ -8392,16 +8388,16 @@
     </row>
     <row r="64" spans="1:12">
       <c r="A64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C64" t="s">
+        <v>102</v>
+      </c>
+      <c r="D64" t="s">
         <v>103</v>
-      </c>
-      <c r="D64" t="s">
-        <v>104</v>
       </c>
       <c r="E64">
         <v>1070</v>
@@ -8430,16 +8426,16 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C65" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D65" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E65">
         <v>2243</v>
@@ -8468,16 +8464,16 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C66" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E66">
         <v>11288</v>
@@ -8506,16 +8502,16 @@
     </row>
     <row r="67" spans="1:12">
       <c r="A67" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C67" t="s">
+        <v>106</v>
+      </c>
+      <c r="D67" t="s">
         <v>107</v>
-      </c>
-      <c r="D67" t="s">
-        <v>108</v>
       </c>
       <c r="E67">
         <v>4745</v>
@@ -8544,16 +8540,16 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B68" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D68" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E68">
         <v>2860</v>
@@ -8582,13 +8578,13 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B69" t="s">
+        <v>109</v>
+      </c>
+      <c r="C69" t="s">
         <v>110</v>
-      </c>
-      <c r="C69" t="s">
-        <v>111</v>
       </c>
       <c r="E69">
         <v>100</v>
@@ -8617,13 +8613,13 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B70" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E70">
         <v>109</v>
@@ -8652,13 +8648,13 @@
     </row>
     <row r="71" spans="1:12">
       <c r="A71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B71" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C71" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -8687,13 +8683,13 @@
     </row>
     <row r="72" spans="1:12">
       <c r="A72" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B72" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C72" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E72">
         <v>496</v>
@@ -8737,50 +8733,50 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
         <v>115</v>
       </c>
-      <c r="B3" t="s">
-        <v>116</v>
-      </c>
       <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
         <v>113</v>
       </c>
-      <c r="D3" t="s">
-        <v>114</v>
-      </c>
       <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>7</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>8</v>
-      </c>
-      <c r="L3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
         <v>30950</v>
@@ -8809,7 +8805,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
         <v>17190</v>
@@ -8838,10 +8834,10 @@
     </row>
     <row r="6" spans="1:12">
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
       </c>
       <c r="E6" s="1">
         <v>2723</v>
@@ -8870,10 +8866,10 @@
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7">
         <v>89</v>
@@ -8902,10 +8898,10 @@
     </row>
     <row r="8" spans="1:12">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -8934,10 +8930,10 @@
     </row>
     <row r="9" spans="1:12">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="1">
         <v>1506</v>
@@ -8966,10 +8962,10 @@
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -8998,10 +8994,10 @@
     </row>
     <row r="11" spans="1:12">
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11">
         <v>80</v>
@@ -9030,10 +9026,10 @@
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12">
         <v>168</v>
@@ -9062,10 +9058,10 @@
     </row>
     <row r="13" spans="1:12">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13">
         <v>24</v>
@@ -9094,10 +9090,10 @@
     </row>
     <row r="14" spans="1:12">
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14">
         <v>916</v>
@@ -9126,10 +9122,10 @@
     </row>
     <row r="15" spans="1:12">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15">
         <v>12</v>
@@ -9158,10 +9154,10 @@
     </row>
     <row r="16" spans="1:12">
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" s="1">
         <v>3494</v>
@@ -9190,10 +9186,10 @@
     </row>
     <row r="17" spans="2:12">
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17">
         <v>935</v>
@@ -9222,10 +9218,10 @@
     </row>
     <row r="18" spans="2:12">
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="1">
         <v>1326</v>
@@ -9254,10 +9250,10 @@
     </row>
     <row r="19" spans="2:12">
       <c r="B19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E19">
         <v>210</v>
@@ -9286,10 +9282,10 @@
     </row>
     <row r="20" spans="2:12">
       <c r="B20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E20">
         <v>546</v>
@@ -9318,10 +9314,10 @@
     </row>
     <row r="21" spans="2:12">
       <c r="B21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E21" s="1">
         <v>12436</v>
@@ -9350,10 +9346,10 @@
     </row>
     <row r="22" spans="2:12">
       <c r="B22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E22" s="1">
         <v>7125</v>
@@ -9382,10 +9378,10 @@
     </row>
     <row r="23" spans="2:12">
       <c r="B23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23" s="1">
         <v>1171</v>
@@ -9414,10 +9410,10 @@
     </row>
     <row r="24" spans="2:12">
       <c r="B24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24">
         <v>58</v>
@@ -9446,10 +9442,10 @@
     </row>
     <row r="25" spans="2:12">
       <c r="B25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E25">
         <v>28</v>
@@ -9478,10 +9474,10 @@
     </row>
     <row r="26" spans="2:12">
       <c r="B26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E26">
         <v>578</v>
@@ -9510,10 +9506,10 @@
     </row>
     <row r="27" spans="2:12">
       <c r="B27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E27">
         <v>102</v>
@@ -9542,10 +9538,10 @@
     </row>
     <row r="28" spans="2:12">
       <c r="B28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E28">
         <v>80</v>
@@ -9574,10 +9570,10 @@
     </row>
     <row r="29" spans="2:12">
       <c r="B29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E29">
         <v>70</v>
@@ -9606,10 +9602,10 @@
     </row>
     <row r="30" spans="2:12">
       <c r="B30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E30">
         <v>38</v>
@@ -9638,10 +9634,10 @@
     </row>
     <row r="31" spans="2:12">
       <c r="B31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -9670,10 +9666,10 @@
     </row>
     <row r="32" spans="2:12">
       <c r="B32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E32">
         <v>144</v>
@@ -9702,7 +9698,7 @@
     </row>
     <row r="33" spans="2:12">
       <c r="B33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -9731,7 +9727,7 @@
     </row>
     <row r="34" spans="2:12">
       <c r="B34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E34" s="1">
         <v>5800</v>
@@ -9760,7 +9756,7 @@
     </row>
     <row r="35" spans="2:12">
       <c r="B35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E35">
         <v>466</v>
@@ -9789,7 +9785,7 @@
     </row>
     <row r="36" spans="2:12">
       <c r="B36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E36" s="1">
         <v>7421</v>
@@ -9818,7 +9814,7 @@
     </row>
     <row r="37" spans="2:12">
       <c r="B37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E37">
         <v>14</v>
@@ -9847,7 +9843,7 @@
     </row>
     <row r="38" spans="2:12">
       <c r="B38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E38">
         <v>170</v>
@@ -9876,7 +9872,7 @@
     </row>
     <row r="39" spans="2:12">
       <c r="B39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E39" s="1">
         <v>51989</v>
@@ -9905,7 +9901,7 @@
     </row>
     <row r="40" spans="2:12">
       <c r="B40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E40">
         <v>503</v>
@@ -9934,7 +9930,7 @@
     </row>
     <row r="41" spans="2:12">
       <c r="B41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E41">
         <v>320</v>
@@ -9963,7 +9959,7 @@
     </row>
     <row r="42" spans="2:12">
       <c r="B42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E42">
         <v>42</v>
@@ -9992,7 +9988,7 @@
     </row>
     <row r="43" spans="2:12">
       <c r="B43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E43" s="1">
         <v>48006</v>
@@ -10021,7 +10017,7 @@
     </row>
     <row r="44" spans="2:12">
       <c r="B44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E44">
         <v>19</v>
@@ -10050,7 +10046,7 @@
     </row>
     <row r="45" spans="2:12">
       <c r="B45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E45" s="1">
         <v>170028</v>
@@ -10079,7 +10075,7 @@
     </row>
     <row r="46" spans="2:12">
       <c r="B46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E46">
         <v>192</v>
@@ -10108,7 +10104,7 @@
     </row>
     <row r="47" spans="2:12">
       <c r="B47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -10137,7 +10133,7 @@
     </row>
     <row r="48" spans="2:12">
       <c r="B48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E48" s="1">
         <v>20148</v>
@@ -10181,10 +10177,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
         <v>120</v>
-      </c>
-      <c r="B1" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -10205,22 +10201,22 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5">
         <v>1993</v>
@@ -10234,50 +10230,50 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" t="s">
         <v>144</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>145</v>
-      </c>
-      <c r="C6" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" t="s">
         <v>147</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>148</v>
-      </c>
-      <c r="D7" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" t="s">
         <v>150</v>
       </c>
-      <c r="B8" t="s">
-        <v>151</v>
-      </c>
       <c r="D8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>